<commit_message>
Short version of input type changer
</commit_message>
<xml_diff>
--- a/Magics.xlsx
+++ b/Magics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Celal\Desktop\DoK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CFFB2D-DC05-47CE-9D9B-2487C733B9A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C91D6F7-EFAA-4407-83A3-82CD97E9BE7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3BA3D8C7-D197-46AB-BC43-4174973D2529}"/>
   </bookViews>
@@ -69,9 +69,6 @@
     <t>The Earthquake</t>
   </si>
   <si>
-    <t>Büyü kullanıldığında seçili olan grid tamamen yok olur.</t>
-  </si>
-  <si>
     <t>The Teleport</t>
   </si>
   <si>
@@ -130,6 +127,9 @@
   </si>
   <si>
     <t>Eklenme Önceliği</t>
+  </si>
+  <si>
+    <t>Büyü kullanıldığında seçili olan grid tamamen yok olur. Grid üstünde herhangi bir şey olmamalı.</t>
   </si>
 </sst>
 </file>
@@ -495,7 +495,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -519,10 +519,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -563,7 +563,7 @@
         <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="F5" s="1">
         <v>1</v>
@@ -571,10 +571,10 @@
     </row>
     <row r="6" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="F6" s="1">
         <v>1</v>
@@ -582,66 +582,66 @@
     </row>
     <row r="7" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="F14" s="1">
         <v>1</v>

</xml_diff>